<commit_message>
Transmission adjustment between symptomatic and non-symptomatic simuls
</commit_message>
<xml_diff>
--- a/Policy inputs.xlsx
+++ b/Policy inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thompson3\Dropbox\COVIDModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A916D804-7A44-4886-8E22-CD0DDC87B199}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B954EC3-448A-4A3F-990E-B57487FF8BCF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C8A0A87-FDC0-44D0-A9C4-C2E3091A8448}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -134,7 +134,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -454,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BF3349-7A93-4850-ABCA-927D8E447EAD}">
-  <dimension ref="B1:K22"/>
+  <dimension ref="B1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -466,7 +466,7 @@
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
@@ -477,7 +477,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -488,7 +488,7 @@
         <v>-0.44</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
@@ -499,7 +499,7 @@
         <v>-0.18</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
@@ -510,7 +510,7 @@
         <v>-0.43</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
@@ -521,7 +521,7 @@
         <v>-0.62</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
@@ -532,7 +532,7 @@
         <v>-0.36</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
@@ -543,7 +543,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C8" s="1">
         <f>AVERAGE(C2:C7)</f>
         <v>-0.55333333333333334</v>
@@ -561,7 +561,7 @@
         <v>0.11385542168674694</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F9" s="3">
         <f>0.8+F8</f>
         <v>0.91385542168674694</v>
@@ -574,13 +574,13 @@
         <v>0.23549999999999999</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="K10">
         <f>1-K9</f>
         <v>0.76449999999999996</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
@@ -594,7 +594,7 @@
         <v>43800</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>9</v>
       </c>
@@ -607,8 +607,14 @@
       <c r="E13" s="7">
         <v>43853</v>
       </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K13">
+        <v>50</v>
+      </c>
+      <c r="L13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>10</v>
       </c>
@@ -622,8 +628,15 @@
       <c r="E14" s="4">
         <v>43929</v>
       </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K14">
+        <f>L14*0.33</f>
+        <v>24.75</v>
+      </c>
+      <c r="L14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
@@ -635,8 +648,20 @@
         <f>D13-D12</f>
         <v>72</v>
       </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K15">
+        <f>K13*K14</f>
+        <v>1237.5</v>
+      </c>
+      <c r="L15">
+        <f>L13*L14</f>
+        <v>3750</v>
+      </c>
+      <c r="M15">
+        <f>SUM(K15:L15)</f>
+        <v>4987.5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>12</v>
       </c>
@@ -649,25 +674,29 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="4">
         <f>C13+90</f>
         <v>44006</v>
       </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <f>SUM(K15:L15)</f>
+        <v>4987.5</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18">
         <f>C17-C13</f>
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C19">
         <f>SUM(C18,C15)</f>
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C20" s="4">
         <v>43936</v>
       </c>
@@ -679,7 +708,7 @@
         <v>43929</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C21">
         <f>C20-C12</f>
         <v>59</v>
@@ -693,7 +722,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C22" s="4">
         <f>C12+147.507</f>
         <v>44024.506999999998</v>

</xml_diff>

<commit_message>
Improvements to stability and reliability in early stages
Now seeded with at least 2 agents and function prevents extinguishment in early stages of model priot to policy triggerday elapse. This prevents early, unrealistic scenarios  (usually < t = 20) that do not reach current real life day status.
</commit_message>
<xml_diff>
--- a/Policy inputs.xlsx
+++ b/Policy inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thompson3\Dropbox\COVIDModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B954EC3-448A-4A3F-990E-B57487FF8BCF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83B9ECE-2B54-4A5A-BC59-D63A6F58BBC6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C8A0A87-FDC0-44D0-A9C4-C2E3091A8448}"/>
   </bookViews>
@@ -457,7 +457,7 @@
   <dimension ref="B1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -714,8 +714,8 @@
         <v>59</v>
       </c>
       <c r="D21">
-        <f>D13-D12</f>
-        <v>72</v>
+        <f>D20-D12</f>
+        <v>91</v>
       </c>
       <c r="E21">
         <f>E13-E12</f>

</xml_diff>

<commit_message>
Track and Trace Implementation - Post Lan
Enables the uses to track contacts from infected people with a certain accuracy and follow-up
</commit_message>
<xml_diff>
--- a/Policy inputs.xlsx
+++ b/Policy inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thompson3\Dropbox\COVIDModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DF7586-D464-4D0C-84D5-4CCDAF2E9D35}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE81EF01-EDC4-4667-9661-CE03F0EAB43D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C8A0A87-FDC0-44D0-A9C4-C2E3091A8448}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Retail and Recreation</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Wuhan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -457,7 +460,7 @@
   <dimension ref="B1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -724,18 +727,29 @@
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C22" s="4">
-        <f>C12+147.507</f>
-        <v>44024.506999999998</v>
+        <v>44014</v>
+      </c>
+      <c r="D22" s="4">
+        <v>44015</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23">
+        <f>D22-D12</f>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C24" s="4">
-        <f>C13+114</f>
-        <v>44030</v>
+        <f>C13+98</f>
+        <v>44014</v>
       </c>
       <c r="D24" s="4">
-        <f>D13+60</f>
-        <v>43978</v>
+        <f>D13+100</f>
+        <v>44018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inclusion of beta distributions for compliance
</commit_message>
<xml_diff>
--- a/Policy inputs.xlsx
+++ b/Policy inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thompson3\Dropbox\COVIDModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD3195E-3BBA-4B45-9910-F4C5F20D8FFE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9464A342-0449-4A7B-A5D3-FEA8D34D7C7D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3765" windowWidth="29040" windowHeight="15840" xr2:uid="{0C8A0A87-FDC0-44D0-A9C4-C2E3091A8448}"/>
+    <workbookView xWindow="3072" yWindow="3072" windowWidth="19200" windowHeight="8520" xr2:uid="{0C8A0A87-FDC0-44D0-A9C4-C2E3091A8448}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Retail and Recreation</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Emissions reduction</t>
   </si>
 </sst>
 </file>
@@ -457,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BF3349-7A93-4850-ABCA-927D8E447EAD}">
-  <dimension ref="B1:M24"/>
+  <dimension ref="B1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,17 +563,27 @@
         <v>0.5692771084337348</v>
       </c>
       <c r="F8" s="3">
-        <f>(1-0.8)*E8</f>
-        <v>0.11385542168674694</v>
+        <f>(1-0.85)*E8</f>
+        <v>8.539156626506024E-2</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="D9">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="E9" s="2">
+        <f>D9/C9</f>
+        <v>0.68357487922705307</v>
+      </c>
       <c r="F9" s="3">
-        <f>0.8+F8</f>
-        <v>0.91385542168674694</v>
-      </c>
-      <c r="G9" t="s">
-        <v>11</v>
+        <f>(1-0.85)*E9</f>
+        <v>0.10253623188405797</v>
       </c>
       <c r="K9">
         <f>0.15*1.57</f>
@@ -578,177 +591,200 @@
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F10" s="3">
+        <f>0.85+F8</f>
+        <v>0.93539156626506026</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
       <c r="K10">
         <f>1-K9</f>
         <v>0.76449999999999996</v>
       </c>
     </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F11" s="3">
+        <f>0.85+F9</f>
+        <v>0.952536231884058</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="6">
-        <v>43877</v>
-      </c>
-      <c r="D12" s="6">
-        <v>43846</v>
-      </c>
-      <c r="E12" s="6">
-        <v>43800</v>
-      </c>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="4">
-        <v>43916</v>
-      </c>
-      <c r="D13" s="4">
-        <v>43918</v>
-      </c>
-      <c r="E13" s="7">
-        <v>43853</v>
-      </c>
-      <c r="K13">
-        <v>50</v>
-      </c>
-      <c r="L13">
-        <v>50</v>
+        <v>8</v>
+      </c>
+      <c r="C13" s="6">
+        <v>43877</v>
+      </c>
+      <c r="D13" s="6">
+        <v>43846</v>
+      </c>
+      <c r="E13" s="6">
+        <v>43800</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="4">
-        <v>43943</v>
+        <v>43916</v>
       </c>
       <c r="D14" s="4">
-        <f>D13+90</f>
-        <v>44008</v>
-      </c>
-      <c r="E14" s="4">
-        <v>43929</v>
+        <v>43918</v>
+      </c>
+      <c r="E14" s="7">
+        <v>43853</v>
       </c>
       <c r="K14">
-        <f>L14*0.33</f>
-        <v>24.75</v>
+        <v>50</v>
       </c>
       <c r="L14">
-        <v>75</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15">
-        <f>C13-C12</f>
-        <v>39</v>
-      </c>
-      <c r="D15">
-        <f>D13-D12</f>
-        <v>72</v>
+        <v>10</v>
+      </c>
+      <c r="C15" s="4">
+        <v>43943</v>
+      </c>
+      <c r="D15" s="4">
+        <f>D14+90</f>
+        <v>44008</v>
+      </c>
+      <c r="E15" s="4">
+        <v>43929</v>
       </c>
       <c r="K15">
-        <f>K13*K14</f>
-        <v>1237.5</v>
+        <f>L15*0.33</f>
+        <v>24.75</v>
       </c>
       <c r="L15">
-        <f>L13*L14</f>
-        <v>3750</v>
-      </c>
-      <c r="M15">
-        <f>SUM(K15:L15)</f>
-        <v>4987.5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <f>C14-C13</f>
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="D16">
         <f>D14-D13</f>
+        <v>72</v>
+      </c>
+      <c r="K16">
+        <f>K14*K15</f>
+        <v>1237.5</v>
+      </c>
+      <c r="L16">
+        <f>L14*L15</f>
+        <v>3750</v>
+      </c>
+      <c r="M16">
+        <f>SUM(K16:L16)</f>
+        <v>4987.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <f>C15-C14</f>
+        <v>27</v>
+      </c>
+      <c r="D17">
+        <f>D15-D14</f>
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C17" s="4">
-        <f>C13+90</f>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C18" s="4">
+        <f>C14+90</f>
         <v>44006</v>
       </c>
-      <c r="L17">
-        <f>SUM(K15:L15)</f>
+      <c r="G18">
+        <f>28.3/41.4 * 0.15</f>
+        <v>0.10253623188405797</v>
+      </c>
+      <c r="L18">
+        <f>SUM(K16:L16)</f>
         <v>4987.5</v>
       </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C18">
-        <f>C17-C13</f>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <f>C18-C14</f>
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C19">
-        <f>SUM(C18,C15)</f>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <f>SUM(C19,C16)</f>
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C20" s="4">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C21" s="4">
         <v>43936</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D21" s="4">
         <v>43937</v>
       </c>
-      <c r="E20" s="4">
-        <f>E13+76</f>
+      <c r="E21" s="4">
+        <f>E14+76</f>
         <v>43929</v>
       </c>
     </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C21">
-        <f>C20-C12</f>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <f>C21-C13</f>
         <v>59</v>
       </c>
-      <c r="D21">
-        <f>D20-D12</f>
+      <c r="D22">
+        <f>D21-D13</f>
         <v>91</v>
       </c>
-      <c r="E21">
-        <f>E14-E12</f>
+      <c r="E22">
+        <f>E15-E13</f>
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C22" s="4">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C23" s="4">
         <v>44014</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D23" s="4">
         <v>44015</v>
       </c>
     </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
         <v>15</v>
       </c>
-      <c r="D23">
-        <f>D22-D12</f>
+      <c r="D24">
+        <f>D23-D13</f>
         <v>169</v>
       </c>
     </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C24" s="4">
-        <f>C13+98</f>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C25" s="4">
+        <f>C14+98</f>
         <v>44014</v>
       </c>
-      <c r="D24" s="4">
-        <f>D13+100</f>
+      <c r="D25" s="4">
+        <f>D14+100</f>
         <v>44018</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to OS_Import function
</commit_message>
<xml_diff>
--- a/Policy inputs.xlsx
+++ b/Policy inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thompson3\Dropbox\COVIDModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9464A342-0449-4A7B-A5D3-FEA8D34D7C7D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF38C2B-67D4-43F0-96BF-B83F964604EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3072" yWindow="3072" windowWidth="19200" windowHeight="8520" xr2:uid="{0C8A0A87-FDC0-44D0-A9C4-C2E3091A8448}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C8A0A87-FDC0-44D0-A9C4-C2E3091A8448}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Retail and Recreation</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Emissions reduction</t>
+  </si>
+  <si>
+    <t>OS Imports</t>
+  </si>
+  <si>
+    <t>Australia</t>
   </si>
 </sst>
 </file>
@@ -136,7 +142,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -145,6 +151,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,19 +467,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BF3349-7A93-4850-ABCA-927D8E447EAD}">
-  <dimension ref="B1:M25"/>
+  <dimension ref="B1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
@@ -483,7 +490,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -494,7 +501,7 @@
         <v>-0.44</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
@@ -505,7 +512,7 @@
         <v>-0.18</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
@@ -516,7 +523,7 @@
         <v>-0.43</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
@@ -527,7 +534,7 @@
         <v>-0.62</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
@@ -538,7 +545,7 @@
         <v>-0.36</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
@@ -549,7 +556,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C8" s="1">
         <f>AVERAGE(C2:C7)</f>
         <v>-0.55333333333333334</v>
@@ -563,11 +570,11 @@
         <v>0.5692771084337348</v>
       </c>
       <c r="F8" s="3">
-        <f>(1-0.85)*E8</f>
-        <v>8.539156626506024E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+        <f>(1-0.85)*(1-E8)</f>
+        <v>6.4608433734939782E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
@@ -582,213 +589,257 @@
         <v>0.68357487922705307</v>
       </c>
       <c r="F9" s="3">
-        <f>(1-0.85)*E9</f>
-        <v>0.10253623188405797</v>
+        <f t="shared" ref="F9:F10" si="0">(1-0.85)*(1-E9)</f>
+        <v>4.7463768115942044E-2</v>
       </c>
       <c r="K9">
         <f>0.15*1.57</f>
         <v>0.23549999999999999</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>96.3</v>
+      </c>
+      <c r="D10">
+        <v>73.2</v>
+      </c>
+      <c r="E10" s="2">
+        <f>D10/C10</f>
+        <v>0.7601246105919004</v>
+      </c>
       <c r="F10" s="3">
-        <f>0.85+F8</f>
-        <v>0.93539156626506026</v>
-      </c>
-      <c r="G10" t="s">
-        <v>11</v>
+        <f>(1-0.85)*(1-E10)</f>
+        <v>3.5981308411214948E-2</v>
       </c>
       <c r="K10">
         <f>1-K9</f>
         <v>0.76449999999999996</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F11" s="3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F12" s="3">
+        <f>0.85+F8</f>
+        <v>0.91460843373493972</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F13" s="3">
         <f>0.85+F9</f>
-        <v>0.952536231884058</v>
-      </c>
-      <c r="G11" t="s">
+        <v>0.89746376811594197</v>
+      </c>
+      <c r="G13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="5" t="s">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F14" s="3">
+        <f>0.85+F10</f>
+        <v>0.88598130841121492</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C16" s="6">
         <v>43877</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D16" s="6">
         <v>43846</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E16" s="6">
         <v>43800</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="s">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C17" s="4">
         <v>43916</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D17" s="4">
         <v>43918</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E17" s="7">
         <v>43853</v>
       </c>
-      <c r="K14">
+      <c r="K17">
         <v>50</v>
       </c>
-      <c r="L14">
+      <c r="L17">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C18" s="4">
         <v>43943</v>
       </c>
-      <c r="D15" s="4">
-        <f>D14+90</f>
+      <c r="D18" s="4">
+        <f>D17+90</f>
         <v>44008</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E18" s="4">
         <v>43929</v>
       </c>
-      <c r="K15">
-        <f>L15*0.33</f>
+      <c r="K18">
+        <f>L18*0.33</f>
         <v>24.75</v>
       </c>
-      <c r="L15">
+      <c r="L18">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="5" t="s">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16">
-        <f>C14-C13</f>
+      <c r="C19">
+        <f>C17-C16</f>
         <v>39</v>
       </c>
-      <c r="D16">
-        <f>D14-D13</f>
+      <c r="D19">
+        <f>D17-D16</f>
         <v>72</v>
       </c>
-      <c r="K16">
-        <f>K14*K15</f>
+      <c r="K19">
+        <f>K17*K18</f>
         <v>1237.5</v>
       </c>
-      <c r="L16">
-        <f>L14*L15</f>
+      <c r="L19">
+        <f>L17*L18</f>
         <v>3750</v>
       </c>
-      <c r="M16">
-        <f>SUM(K16:L16)</f>
+      <c r="M19">
+        <f>SUM(K19:L19)</f>
         <v>4987.5</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="5" t="s">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C17">
-        <f>C15-C14</f>
+      <c r="C20">
+        <f>C18-C17</f>
         <v>27</v>
       </c>
-      <c r="D17">
-        <f>D15-D14</f>
+      <c r="D20">
+        <f>D18-D17</f>
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C18" s="4">
-        <f>C14+90</f>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C21" s="4">
+        <f>C17+90</f>
         <v>44006</v>
       </c>
-      <c r="G18">
+      <c r="G21">
         <f>28.3/41.4 * 0.15</f>
         <v>0.10253623188405797</v>
       </c>
-      <c r="L18">
-        <f>SUM(K16:L16)</f>
+      <c r="L21">
+        <f>SUM(K19:L19)</f>
         <v>4987.5</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C19">
-        <f>C18-C14</f>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <f>C21-C17</f>
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C20">
-        <f>SUM(C19,C16)</f>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <f>SUM(C22,C19)</f>
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C21" s="4">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C24" s="4">
         <v>43936</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D24" s="4">
         <v>43937</v>
       </c>
-      <c r="E21" s="4">
-        <f>E14+76</f>
+      <c r="E24" s="4">
+        <f>E17+76</f>
         <v>43929</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C22">
-        <f>C21-C13</f>
+      <c r="K24" t="s">
+        <v>17</v>
+      </c>
+      <c r="L24" t="s">
+        <v>18</v>
+      </c>
+      <c r="M24" s="8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <f>C24-C16</f>
         <v>59</v>
       </c>
-      <c r="D22">
-        <f>D21-D13</f>
+      <c r="D25">
+        <f>D24-D16</f>
         <v>91</v>
       </c>
-      <c r="E22">
-        <f>E15-E13</f>
+      <c r="E25">
+        <f>E18-E16</f>
         <v>129</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C23" s="4">
+      <c r="L25" t="s">
+        <v>1</v>
+      </c>
+      <c r="M25" s="8">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C26" s="4">
         <v>44014</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D26" s="4">
         <v>44015</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
         <v>15</v>
       </c>
-      <c r="D24">
-        <f>D23-D13</f>
+      <c r="D27">
+        <f>D26-D16</f>
         <v>169</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C25" s="4">
-        <f>C14+98</f>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C28" s="4">
+        <f>C17+98</f>
         <v>44014</v>
       </c>
-      <c r="D25" s="4">
-        <f>D14+100</f>
+      <c r="D28" s="4">
+        <f>D17+100</f>
         <v>44018</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C30" s="4">
+        <f>C17+60</f>
+        <v>43976</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor tweaks to OS
</commit_message>
<xml_diff>
--- a/Policy inputs.xlsx
+++ b/Policy inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thompson3\Dropbox\COVIDModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF38C2B-67D4-43F0-96BF-B83F964604EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6381989F-0210-4AEC-8C0C-699989CEE358}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C8A0A87-FDC0-44D0-A9C4-C2E3091A8448}"/>
   </bookViews>
@@ -469,7 +469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BF3349-7A93-4850-ABCA-927D8E447EAD}">
   <dimension ref="B1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
@@ -589,7 +589,7 @@
         <v>0.68357487922705307</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" ref="F9:F10" si="0">(1-0.85)*(1-E9)</f>
+        <f t="shared" ref="F9" si="0">(1-0.85)*(1-E9)</f>
         <v>4.7463768115942044E-2</v>
       </c>
       <c r="K9">

</xml_diff>

<commit_message>
Adjustment to mean contacts calculation
</commit_message>
<xml_diff>
--- a/Policy inputs.xlsx
+++ b/Policy inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thompson3\Dropbox\COVIDModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BAC295-9F76-46AE-ACAE-330670EF5F17}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F060EE7-51DB-4CB4-B37C-669DB8FA3199}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C8A0A87-FDC0-44D0-A9C4-C2E3091A8448}"/>
   </bookViews>
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BF3349-7A93-4850-ABCA-927D8E447EAD}">
   <dimension ref="B1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>